<commit_message>
Fix build issue: remove fix_database from deploy and rely on migrations
</commit_message>
<xml_diff>
--- a/output/user_output.xlsx
+++ b/output/user_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="257">
   <si>
     <t>part_number</t>
   </si>
@@ -193,331 +193,334 @@
     <t>source_file</t>
   </si>
   <si>
-    <t>P0016</t>
-  </si>
-  <si>
-    <t>P0017</t>
-  </si>
-  <si>
-    <t>P0018</t>
-  </si>
-  <si>
-    <t>P0019</t>
-  </si>
-  <si>
-    <t>P0020</t>
-  </si>
-  <si>
-    <t>NP010</t>
-  </si>
-  <si>
-    <t>INV007</t>
-  </si>
-  <si>
-    <t>INV008</t>
-  </si>
-  <si>
-    <t>INV009</t>
-  </si>
-  <si>
-    <t>INV010</t>
-  </si>
-  <si>
-    <t>1308.0</t>
-  </si>
-  <si>
-    <t>1895.0</t>
-  </si>
-  <si>
-    <t>474.0</t>
-  </si>
-  <si>
-    <t>1666.0</t>
-  </si>
-  <si>
-    <t>386.0</t>
-  </si>
-  <si>
-    <t>V243</t>
-  </si>
-  <si>
-    <t>V512</t>
-  </si>
-  <si>
-    <t>V561</t>
-  </si>
-  <si>
-    <t>V885</t>
-  </si>
-  <si>
-    <t>V364</t>
+    <t>P0006</t>
+  </si>
+  <si>
+    <t>P0007</t>
+  </si>
+  <si>
+    <t>P0008</t>
+  </si>
+  <si>
+    <t>P0009</t>
+  </si>
+  <si>
+    <t>P0010</t>
+  </si>
+  <si>
+    <t>NP004</t>
+  </si>
+  <si>
+    <t>NP005</t>
+  </si>
+  <si>
+    <t>NP006</t>
+  </si>
+  <si>
+    <t>INV003</t>
+  </si>
+  <si>
+    <t>INV004</t>
+  </si>
+  <si>
+    <t>1345.0</t>
+  </si>
+  <si>
+    <t>88.0</t>
+  </si>
+  <si>
+    <t>422.0</t>
+  </si>
+  <si>
+    <t>1326.0</t>
+  </si>
+  <si>
+    <t>445.0</t>
+  </si>
+  <si>
+    <t>V366</t>
+  </si>
+  <si>
+    <t>V517</t>
+  </si>
+  <si>
+    <t>V976</t>
+  </si>
+  <si>
+    <t>V190</t>
+  </si>
+  <si>
+    <t>V565</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>96119023.0</t>
+  </si>
+  <si>
+    <t>45211434.0</t>
+  </si>
+  <si>
+    <t>14735717.0</t>
+  </si>
+  <si>
+    <t>81563511.0</t>
+  </si>
+  <si>
+    <t>38610938.0</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Bearing</t>
+  </si>
+  <si>
+    <t>Hydraulic</t>
+  </si>
+  <si>
+    <t>Pipe Fitting</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>19847109.0</t>
-  </si>
-  <si>
-    <t>43167078.0</t>
-  </si>
-  <si>
-    <t>83296537.0</t>
-  </si>
-  <si>
-    <t>44248190.0</t>
-  </si>
-  <si>
-    <t>33116006.0</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>0.83</t>
-  </si>
-  <si>
-    <t>0.59</t>
-  </si>
-  <si>
-    <t>Bracket</t>
+    <t>1794.14</t>
+  </si>
+  <si>
+    <t>3251.38</t>
+  </si>
+  <si>
+    <t>2911.33</t>
+  </si>
+  <si>
+    <t>1458.17</t>
+  </si>
+  <si>
+    <t>2096.8</t>
+  </si>
+  <si>
+    <t>2787.32</t>
+  </si>
+  <si>
+    <t>101.62</t>
+  </si>
+  <si>
+    <t>EA</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>MTR</t>
+  </si>
+  <si>
+    <t>Verify with drawing</t>
+  </si>
+  <si>
+    <t>Check interference</t>
+  </si>
+  <si>
+    <t>Update model</t>
+  </si>
+  <si>
+    <t>SS304 Stepper Motor 45x52 mm</t>
+  </si>
+  <si>
+    <t>Brass DC Motor 20x162 mm</t>
+  </si>
+  <si>
+    <t>Aluminum Roller Bearing 39x19 mm</t>
+  </si>
+  <si>
+    <t>SS316 Coupler 9x14 mm</t>
+  </si>
+  <si>
+    <t>Aluminum Elbow 50x198 mm</t>
+  </si>
+  <si>
+    <t>DRW0006</t>
+  </si>
+  <si>
+    <t>DRW0007</t>
+  </si>
+  <si>
+    <t>DRW0008</t>
+  </si>
+  <si>
+    <t>DRW0009</t>
+  </si>
+  <si>
+    <t>DRW0010</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>BOX</t>
+  </si>
+  <si>
+    <t>SS304</t>
+  </si>
+  <si>
+    <t>SS316</t>
+  </si>
+  <si>
+    <t>EN8</t>
+  </si>
+  <si>
+    <t>Zinc Plated</t>
+  </si>
+  <si>
+    <t>Anodized</t>
+  </si>
+  <si>
+    <t>Brass</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>Nylon</t>
+  </si>
+  <si>
+    <t>Plastic</t>
+  </si>
+  <si>
+    <t>35x150 mm</t>
+  </si>
+  <si>
+    <t>18x45 mm</t>
+  </si>
+  <si>
+    <t>10x32 mm</t>
+  </si>
+  <si>
+    <t>22x65 mm</t>
+  </si>
+  <si>
+    <t>14x90 mm</t>
+  </si>
+  <si>
+    <t>39x90 mm</t>
+  </si>
+  <si>
+    <t>39x46 mm</t>
+  </si>
+  <si>
+    <t>27x117 mm</t>
+  </si>
+  <si>
+    <t>22x37 mm</t>
+  </si>
+  <si>
+    <t>24x62 mm</t>
+  </si>
+  <si>
+    <t>05-06-2023</t>
+  </si>
+  <si>
+    <t>20-11-2024</t>
+  </si>
+  <si>
+    <t>04-04-2023</t>
+  </si>
+  <si>
+    <t>18-09-2024</t>
+  </si>
+  <si>
+    <t>11-02-2021</t>
+  </si>
+  <si>
+    <t>Brass Roller Bearing 35x150 mm</t>
+  </si>
+  <si>
+    <t>Steel Hex Bolt 18x45 mm</t>
+  </si>
+  <si>
+    <t>SS304 Washer 10x32 mm</t>
+  </si>
+  <si>
+    <t>Aluminum Pipe Coupling 22x65 mm</t>
+  </si>
+  <si>
+    <t>Nylon Relay Bracket 14x90 mm</t>
+  </si>
+  <si>
+    <t>Steel Screw 39x90 mm</t>
+  </si>
+  <si>
+    <t>Plastic Valve 39x46 mm</t>
+  </si>
+  <si>
+    <t>Aluminum Relay 27x117 mm</t>
+  </si>
+  <si>
+    <t>Steel Solenoid 22x37 mm</t>
+  </si>
+  <si>
+    <t>Brass Gear Wheel 24x62 mm</t>
   </si>
   <si>
     <t>Fastener</t>
   </si>
   <si>
-    <t>Hydraulic</t>
-  </si>
-  <si>
     <t>Electrical</t>
   </si>
   <si>
-    <t>2629.56</t>
-  </si>
-  <si>
-    <t>4140.3</t>
-  </si>
-  <si>
-    <t>782.92</t>
-  </si>
-  <si>
-    <t>783.19</t>
-  </si>
-  <si>
-    <t>1884.55</t>
-  </si>
-  <si>
-    <t>434.26</t>
-  </si>
-  <si>
-    <t>352.85</t>
-  </si>
-  <si>
-    <t>2085.35</t>
-  </si>
-  <si>
-    <t>1486.24</t>
-  </si>
-  <si>
-    <t>MTR</t>
-  </si>
-  <si>
-    <t>EA</t>
-  </si>
-  <si>
-    <t>Check interference</t>
-  </si>
-  <si>
-    <t>Verify with drawing</t>
-  </si>
-  <si>
-    <t>Update model</t>
-  </si>
-  <si>
-    <t>Brass U Bracket 12x40 mm</t>
-  </si>
-  <si>
-    <t>Steel Nut 15x200 mm</t>
-  </si>
-  <si>
-    <t>SS316 U Bracket 42x199 mm</t>
-  </si>
-  <si>
-    <t>Aluminum Valve 47x42 mm</t>
-  </si>
-  <si>
-    <t>Steel Connector 24x81 mm</t>
-  </si>
-  <si>
-    <t>DRW0016</t>
-  </si>
-  <si>
-    <t>DRW0017</t>
-  </si>
-  <si>
-    <t>DRW0018</t>
-  </si>
-  <si>
-    <t>DRW0019</t>
-  </si>
-  <si>
-    <t>DRW0020</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>BOX</t>
-  </si>
-  <si>
-    <t>KG</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>SS304</t>
-  </si>
-  <si>
-    <t>Polished</t>
-  </si>
-  <si>
-    <t>SS316</t>
-  </si>
-  <si>
-    <t>Steel</t>
-  </si>
-  <si>
-    <t>Brass</t>
-  </si>
-  <si>
-    <t>Nylon</t>
-  </si>
-  <si>
-    <t>Aluminum</t>
-  </si>
-  <si>
-    <t>Plastic</t>
-  </si>
-  <si>
-    <t>25x120 mm</t>
-  </si>
-  <si>
-    <t>22x75 mm</t>
-  </si>
-  <si>
-    <t>20x60 mm</t>
-  </si>
-  <si>
-    <t>28x110 mm</t>
-  </si>
-  <si>
-    <t>15x85 mm</t>
-  </si>
-  <si>
-    <t>23x138 mm</t>
-  </si>
-  <si>
-    <t>29x34 mm</t>
-  </si>
-  <si>
-    <t>12x91 mm</t>
-  </si>
-  <si>
-    <t>31x90 mm</t>
-  </si>
-  <si>
-    <t>28x122 mm</t>
-  </si>
-  <si>
-    <t>20-01-2022</t>
-  </si>
-  <si>
-    <t>07-03-2024</t>
-  </si>
-  <si>
-    <t>12-06-2024</t>
-  </si>
-  <si>
-    <t>12-05-2024</t>
-  </si>
-  <si>
-    <t>23-11-2024</t>
-  </si>
-  <si>
-    <t>SS316 Bracket 25x120 mm</t>
-  </si>
-  <si>
-    <t>Steel Flange 22x75 mm</t>
-  </si>
-  <si>
-    <t>Brass Elbow 20x60 mm</t>
-  </si>
-  <si>
-    <t>Nylon Motor Housing 28x110 mm</t>
-  </si>
-  <si>
-    <t>Aluminum L Bracket 15x85 mm</t>
-  </si>
-  <si>
-    <t>Aluminum Valve 23x138 mm</t>
-  </si>
-  <si>
-    <t>Plastic Fuse Holder 29x34 mm</t>
-  </si>
-  <si>
-    <t>Aluminum Coupler 12x91 mm</t>
-  </si>
-  <si>
-    <t>Steel Coupler 31x90 mm</t>
-  </si>
-  <si>
-    <t>Steel Gear Wheel 28x122 mm</t>
-  </si>
-  <si>
-    <t>Pipe Fitting</t>
-  </si>
-  <si>
-    <t>Motor</t>
-  </si>
-  <si>
     <t>Valve</t>
   </si>
   <si>
-    <t>Fuse</t>
+    <t>Solenoid</t>
   </si>
   <si>
     <t>Gear</t>
   </si>
   <si>
+    <t>Check vendor lead time</t>
+  </si>
+  <si>
+    <t>High stock movement</t>
+  </si>
+  <si>
     <t>Part used frequently</t>
   </si>
   <si>
-    <t>High stock movement</t>
-  </si>
-  <si>
     <t>Consider alternate sourcing</t>
   </si>
   <si>
-    <t>25-01-2022</t>
-  </si>
-  <si>
-    <t>16-04-2021</t>
-  </si>
-  <si>
-    <t>22-10-2020</t>
-  </si>
-  <si>
-    <t>07-07-2023</t>
-  </si>
-  <si>
-    <t>25-05-2020</t>
+    <t>05-09-2023</t>
+  </si>
+  <si>
+    <t>24-02-2021</t>
+  </si>
+  <si>
+    <t>20-08-2024</t>
+  </si>
+  <si>
+    <t>16-04-2024</t>
+  </si>
+  <si>
+    <t>26-01-2024</t>
+  </si>
+  <si>
+    <t>1000.0</t>
   </si>
   <si>
     <t>2000.0</t>
@@ -526,31 +529,28 @@
     <t>3000.0</t>
   </si>
   <si>
+    <t>INR</t>
+  </si>
+  <si>
     <t>EUR</t>
   </si>
   <si>
     <t>USD</t>
   </si>
   <si>
-    <t>INR</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
     <t>Low</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>Checked Out</t>
   </si>
   <si>
     <t>Checked In</t>
   </si>
   <si>
-    <t>Goods Damaged</t>
+    <t>Warranty Included</t>
   </si>
   <si>
     <t>Approved</t>
@@ -562,61 +562,58 @@
     <t>Under Review</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>ROH</t>
+  </si>
+  <si>
+    <t>FERT</t>
+  </si>
+  <si>
     <t>HALB</t>
   </si>
   <si>
-    <t>FERT</t>
-  </si>
-  <si>
-    <t>ROH</t>
-  </si>
-  <si>
-    <t>39.0</t>
-  </si>
-  <si>
-    <t>42.0</t>
-  </si>
-  <si>
-    <t>27.0</t>
-  </si>
-  <si>
-    <t>9.14</t>
-  </si>
-  <si>
-    <t>6.14</t>
-  </si>
-  <si>
-    <t>8.63</t>
-  </si>
-  <si>
-    <t>3.65</t>
-  </si>
-  <si>
-    <t>10.9</t>
-  </si>
-  <si>
-    <t>INV2006</t>
-  </si>
-  <si>
-    <t>INV2007</t>
-  </si>
-  <si>
-    <t>INV2008</t>
-  </si>
-  <si>
-    <t>INV2009</t>
+    <t>22.0</t>
+  </si>
+  <si>
+    <t>60.0</t>
+  </si>
+  <si>
+    <t>64.0</t>
+  </si>
+  <si>
+    <t>3.42</t>
+  </si>
+  <si>
+    <t>13.71</t>
+  </si>
+  <si>
+    <t>12.67</t>
+  </si>
+  <si>
+    <t>2.63</t>
+  </si>
+  <si>
+    <t>4.46</t>
+  </si>
+  <si>
+    <t>INV2002</t>
+  </si>
+  <si>
+    <t>INV2003</t>
   </si>
   <si>
     <t>IAM</t>
   </si>
   <si>
-    <t>STEP</t>
-  </si>
-  <si>
-    <t>IPT</t>
-  </si>
-  <si>
-    <t>SL14</t>
+    <t>DWG</t>
+  </si>
+  <si>
+    <t>SL49</t>
+  </si>
+  <si>
+    <t>SL10</t>
   </si>
   <si>
     <t>SL6</t>
@@ -625,133 +622,124 @@
     <t>SL24</t>
   </si>
   <si>
-    <t>SL23</t>
-  </si>
-  <si>
-    <t>199</t>
-  </si>
-  <si>
-    <t>378</t>
-  </si>
-  <si>
-    <t>484</t>
-  </si>
-  <si>
-    <t>360</t>
+    <t>SL20</t>
+  </si>
+  <si>
+    <t>275</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>1.0</t>
   </si>
   <si>
     <t>2.0</t>
   </si>
   <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>Suresh</t>
+    <t>Meena</t>
   </si>
   <si>
     <t>John</t>
   </si>
   <si>
+    <t>Kumar</t>
+  </si>
+  <si>
     <t>Priya</t>
   </si>
   <si>
-    <t>Kumar</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
-    <t>22.76</t>
-  </si>
-  <si>
-    <t>3.11</t>
-  </si>
-  <si>
-    <t>23.35</t>
-  </si>
-  <si>
-    <t>7.08</t>
-  </si>
-  <si>
-    <t>7.64</t>
+    <t>19.31</t>
+  </si>
+  <si>
+    <t>6.36</t>
+  </si>
+  <si>
+    <t>14.85</t>
+  </si>
+  <si>
+    <t>24.42</t>
+  </si>
+  <si>
+    <t>8.78</t>
+  </si>
+  <si>
+    <t>Batch</t>
   </si>
   <si>
     <t>Standard</t>
   </si>
   <si>
-    <t>Batch</t>
-  </si>
-  <si>
-    <t>±0.25 mm</t>
-  </si>
-  <si>
-    <t>±0.63 mm</t>
-  </si>
-  <si>
-    <t>±0.28 mm</t>
-  </si>
-  <si>
-    <t>±0.33 mm</t>
-  </si>
-  <si>
-    <t>±0.56 mm</t>
-  </si>
-  <si>
-    <t>48.0</t>
-  </si>
-  <si>
-    <t>83.0</t>
+    <t>±0.86 mm</t>
+  </si>
+  <si>
+    <t>±0.68 mm</t>
+  </si>
+  <si>
+    <t>±0.49 mm</t>
+  </si>
+  <si>
+    <t>±0.39 mm</t>
+  </si>
+  <si>
+    <t>±0.64 mm</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>28.0</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>2024-02-14</t>
-  </si>
-  <si>
-    <t>2024-11-28</t>
-  </si>
-  <si>
-    <t>2024-12-07</t>
-  </si>
-  <si>
-    <t>2024-10-05</t>
-  </si>
-  <si>
-    <t>2024-08-04</t>
-  </si>
-  <si>
-    <t>2024-05-19</t>
-  </si>
-  <si>
-    <t>2024-05-15</t>
-  </si>
-  <si>
-    <t>2024-12-15</t>
-  </si>
-  <si>
-    <t>P0016.ipt</t>
-  </si>
-  <si>
-    <t>P0017.ipt</t>
-  </si>
-  <si>
-    <t>P0018.ipt</t>
-  </si>
-  <si>
-    <t>P0019.ipt</t>
-  </si>
-  <si>
-    <t>P0020.ipt</t>
-  </si>
-  <si>
-    <t>[{"source_system": "sap", "source_file": "sap_master_mock.xlsx"}, {"source_system": "vault", "source_file": "vault_mock_aligned.xlsx"}, {"source_system": "powerbi", "source_file": "powerbi_mock_aligned.xlsx"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"source_system": "invoices", "source_file": "invoice_mock_newparts.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}, {"source_system": "user", "source_file": "diagram 4.pdf"}]</t>
+    <t>2024-11-27</t>
+  </si>
+  <si>
+    <t>2024-01-02</t>
+  </si>
+  <si>
+    <t>2024-01-24</t>
+  </si>
+  <si>
+    <t>2024-06-05</t>
+  </si>
+  <si>
+    <t>P0006.ipt</t>
+  </si>
+  <si>
+    <t>P0007.ipt</t>
+  </si>
+  <si>
+    <t>P0008.ipt</t>
+  </si>
+  <si>
+    <t>P0009.ipt</t>
+  </si>
+  <si>
+    <t>P0010.ipt</t>
+  </si>
+  <si>
+    <t>[{"source_system": "sap", "source_file": "sap_master_mock.xlsx"}, {"source_system": "vault", "source_file": "vault_mock_aligned.xlsx"}, {"source_system": "powerbi", "source_file": "powerbi_mock_aligned.xlsx"}, {"source_system": "user", "source_file": "diagram2.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"source": "user", "file": "diagram 7.pdf", "description": "Steel Screw 39x90 mm"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source": "user", "file": "diagram 7.pdf", "description": "Steel Screw 39x90 mm"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source": "user", "file": "diagram 7.pdf", "description": "Steel Screw 39x90 mm"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}]</t>
+  </si>
+  <si>
+    <t>[{"source_system": "invoices", "source_file": "invoice_mock_newparts.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}]</t>
+  </si>
+  <si>
+    <t>Released</t>
   </si>
   <si>
     <t>In Work</t>
@@ -760,46 +748,43 @@
     <t>Obsolete</t>
   </si>
   <si>
-    <t>Prime Engineering</t>
+    <t>Global Metals</t>
   </si>
   <si>
     <t>MechSolutions</t>
   </si>
   <si>
+    <t>ElectroWorks</t>
+  </si>
+  <si>
     <t>ABC Industries</t>
   </si>
   <si>
-    <t>ElectroWorks</t>
+    <t>Alpha Metals</t>
   </si>
   <si>
     <t>TruParts</t>
   </si>
   <si>
-    <t>Alpha Metals</t>
-  </si>
-  <si>
-    <t>Zenith Engineers</t>
-  </si>
-  <si>
-    <t>part_0016.step</t>
-  </si>
-  <si>
-    <t>part_0017.step</t>
-  </si>
-  <si>
-    <t>part_0018.step</t>
-  </si>
-  <si>
-    <t>part_0019.step</t>
-  </si>
-  <si>
-    <t>part_0020.step</t>
+    <t>part_0006.step</t>
+  </si>
+  <si>
+    <t>part_0007.step</t>
+  </si>
+  <si>
+    <t>part_0008.step</t>
+  </si>
+  <si>
+    <t>part_0009.step</t>
+  </si>
+  <si>
+    <t>part_0010.step</t>
   </si>
   <si>
     <t>user</t>
   </si>
   <si>
-    <t>diagram 4.pdf</t>
+    <t>diagram2.pdf</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1336,7 @@
         <v>59</v>
       </c>
       <c r="B2" s="2">
-        <v>46004.72183795925</v>
+        <v>46004.72246635323</v>
       </c>
       <c r="C2" t="s">
         <v>69</v>
@@ -1363,50 +1348,59 @@
         <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J2" t="s">
         <v>94</v>
       </c>
       <c r="K2" t="s">
-        <v>103</v>
+        <v>101</v>
+      </c>
+      <c r="L2" t="s">
+        <v>104</v>
       </c>
       <c r="M2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P2" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q2" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" t="s">
-        <v>121</v>
+      <c r="R2" t="s">
+        <v>122</v>
       </c>
       <c r="S2" t="s">
         <v>124</v>
       </c>
       <c r="T2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="U2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="V2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="W2" t="s">
         <v>90</v>
       </c>
+      <c r="X2" t="s">
+        <v>159</v>
+      </c>
       <c r="Y2" t="s">
         <v>163</v>
       </c>
@@ -1414,10 +1408,10 @@
         <v>168</v>
       </c>
       <c r="AA2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AB2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AC2" t="s">
         <v>176</v>
@@ -1426,61 +1420,64 @@
         <v>179</v>
       </c>
       <c r="AF2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="AI2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AK2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AL2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="AO2" t="s">
         <v>90</v>
       </c>
       <c r="AP2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="AQ2" t="s">
-        <v>214</v>
+        <v>117</v>
       </c>
       <c r="AR2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AS2" t="s">
+        <v>218</v>
+      </c>
+      <c r="AT2" t="s">
         <v>220</v>
       </c>
-      <c r="AT2" t="s">
-        <v>222</v>
+      <c r="AU2" t="s">
+        <v>225</v>
       </c>
       <c r="AX2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BA2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="BB2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="BC2" t="s">
-        <v>181</v>
+        <v>241</v>
       </c>
       <c r="BD2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="BE2" t="s">
+        <v>250</v>
+      </c>
+      <c r="BF2" t="s">
         <v>255</v>
       </c>
-      <c r="BF2" t="s">
-        <v>260</v>
-      </c>
       <c r="BG2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:59">
@@ -1488,7 +1485,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="2">
-        <v>46004.72183795925</v>
+        <v>46004.72246635323</v>
       </c>
       <c r="C3" t="s">
         <v>70</v>
@@ -1497,142 +1494,142 @@
         <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J3" t="s">
         <v>95</v>
       </c>
       <c r="K3" t="s">
-        <v>103</v>
-      </c>
-      <c r="L3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="M3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O3" t="s">
+        <v>117</v>
+      </c>
+      <c r="P3" t="s">
         <v>118</v>
       </c>
-      <c r="P3" t="s">
-        <v>119</v>
-      </c>
       <c r="Q3" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="R3" t="s">
+        <v>123</v>
       </c>
       <c r="S3" t="s">
         <v>125</v>
       </c>
       <c r="T3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="V3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="W3" t="s">
-        <v>155</v>
-      </c>
-      <c r="X3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="Y3" t="s">
         <v>164</v>
       </c>
       <c r="Z3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AA3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="AB3" t="s">
         <v>174</v>
       </c>
       <c r="AC3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AE3" t="s">
         <v>180</v>
       </c>
       <c r="AF3" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="AG3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AH3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AI3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AK3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AL3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AN3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AO3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AP3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="AQ3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AR3" t="s">
         <v>214</v>
       </c>
-      <c r="AR3" t="s">
-        <v>216</v>
-      </c>
       <c r="AS3" t="s">
+        <v>219</v>
+      </c>
+      <c r="AT3" t="s">
         <v>221</v>
       </c>
-      <c r="AT3" t="s">
-        <v>223</v>
+      <c r="AU3" t="s">
+        <v>226</v>
       </c>
       <c r="AX3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BA3" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="BB3" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="BC3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="BD3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="BE3" t="s">
+        <v>251</v>
+      </c>
+      <c r="BF3" t="s">
+        <v>255</v>
+      </c>
+      <c r="BG3" t="s">
         <v>256</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>260</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:59">
@@ -1640,7 +1637,7 @@
         <v>61</v>
       </c>
       <c r="B4" s="2">
-        <v>46004.72183795925</v>
+        <v>46004.72246635323</v>
       </c>
       <c r="C4" t="s">
         <v>71</v>
@@ -1652,73 +1649,73 @@
         <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
         <v>90</v>
       </c>
       <c r="I4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
         <v>96</v>
       </c>
       <c r="K4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>121</v>
+      </c>
+      <c r="S4" t="s">
         <v>119</v>
       </c>
-      <c r="Q4" t="s">
-        <v>122</v>
-      </c>
-      <c r="R4" t="s">
-        <v>123</v>
-      </c>
-      <c r="S4" t="s">
-        <v>126</v>
-      </c>
       <c r="T4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="U4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="W4" t="s">
-        <v>155</v>
+        <v>154</v>
+      </c>
+      <c r="X4" t="s">
+        <v>160</v>
       </c>
       <c r="Y4" t="s">
         <v>165</v>
       </c>
       <c r="Z4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="AA4" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="AB4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="AC4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="AE4" t="s">
         <v>179</v>
@@ -1727,64 +1724,61 @@
         <v>79</v>
       </c>
       <c r="AG4" t="s">
-        <v>184</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AI4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AK4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AL4" t="s">
-        <v>202</v>
+        <v>200</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>206</v>
       </c>
       <c r="AO4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AP4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="AQ4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AR4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="AS4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AT4" t="s">
-        <v>224</v>
-      </c>
-      <c r="AU4" t="s">
+        <v>222</v>
+      </c>
+      <c r="AX4" t="s">
         <v>227</v>
       </c>
-      <c r="AX4" t="s">
-        <v>229</v>
-      </c>
       <c r="BA4" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="BB4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="BC4" t="s">
+        <v>181</v>
+      </c>
+      <c r="BD4" t="s">
         <v>246</v>
       </c>
-      <c r="BD4" t="s">
-        <v>250</v>
-      </c>
       <c r="BE4" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="BF4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="BG4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:59">
@@ -1792,7 +1786,7 @@
         <v>62</v>
       </c>
       <c r="B5" s="2">
-        <v>46004.72183795925</v>
+        <v>46004.72246635323</v>
       </c>
       <c r="C5" t="s">
         <v>72</v>
@@ -1804,55 +1798,58 @@
         <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="G5" t="s">
+        <v>88</v>
       </c>
       <c r="H5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="J5" t="s">
         <v>97</v>
       </c>
       <c r="K5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O5" t="s">
+        <v>117</v>
+      </c>
+      <c r="P5" t="s">
         <v>118</v>
       </c>
-      <c r="P5" t="s">
-        <v>120</v>
-      </c>
       <c r="Q5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="R5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="U5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="V5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="W5" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="X5" t="s">
         <v>161</v>
@@ -1861,79 +1858,82 @@
         <v>166</v>
       </c>
       <c r="Z5" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="AA5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AB5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AC5" t="s">
         <v>177</v>
       </c>
       <c r="AE5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AF5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG5" t="s">
-        <v>183</v>
+        <v>185</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>187</v>
       </c>
       <c r="AI5" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AK5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AL5" t="s">
         <v>201</v>
       </c>
       <c r="AN5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AO5" t="s">
-        <v>156</v>
+        <v>92</v>
       </c>
       <c r="AP5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AQ5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AR5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AS5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AT5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AX5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BA5" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="BB5" t="s">
+        <v>237</v>
+      </c>
+      <c r="BC5" t="s">
         <v>243</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BD5" t="s">
         <v>247</v>
       </c>
-      <c r="BD5" t="s">
-        <v>251</v>
-      </c>
       <c r="BE5" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="BF5" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="BG5" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:59">
@@ -1941,7 +1941,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="2">
-        <v>46004.72183795925</v>
+        <v>46004.72246635323</v>
       </c>
       <c r="C6" t="s">
         <v>73</v>
@@ -1950,58 +1950,55 @@
         <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" t="s">
         <v>93</v>
-      </c>
-      <c r="I6" t="s">
-        <v>80</v>
       </c>
       <c r="J6" t="s">
         <v>98</v>
       </c>
       <c r="K6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N6" t="s">
+        <v>116</v>
+      </c>
+      <c r="O6" t="s">
         <v>117</v>
       </c>
-      <c r="O6" t="s">
-        <v>118</v>
-      </c>
       <c r="P6" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q6" t="s">
         <v>119</v>
       </c>
-      <c r="Q6" t="s">
-        <v>122</v>
-      </c>
       <c r="S6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="U6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="V6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="W6" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="X6" t="s">
         <v>162</v>
@@ -2013,79 +2010,76 @@
         <v>168</v>
       </c>
       <c r="AA6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AB6" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="AC6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AE6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AF6" t="s">
         <v>80</v>
       </c>
       <c r="AG6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="AH6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="AI6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AK6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="AL6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AO6" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="AP6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="AQ6" t="s">
-        <v>118</v>
+        <v>212</v>
       </c>
       <c r="AR6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AS6" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AT6" t="s">
-        <v>226</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AX6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BA6" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="BB6" t="s">
+        <v>237</v>
+      </c>
+      <c r="BC6" t="s">
         <v>243</v>
       </c>
-      <c r="BC6" t="s">
-        <v>247</v>
-      </c>
       <c r="BD6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="BE6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="BF6" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="BG6" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:59">
@@ -2093,34 +2087,34 @@
         <v>64</v>
       </c>
       <c r="B7" s="2">
-        <v>46004.72183795925</v>
+        <v>46004.70114318176</v>
       </c>
       <c r="S7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="T7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="V7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="W7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AO7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AX7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="BB7" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="BF7" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="BG7" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:59">
@@ -2128,55 +2122,34 @@
         <v>65</v>
       </c>
       <c r="B8" s="2">
-        <v>46004.72183795925</v>
-      </c>
-      <c r="J8" t="s">
-        <v>99</v>
+        <v>46004.70114318176</v>
       </c>
       <c r="S8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="V8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="W8" t="s">
-        <v>158</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>172</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>193</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>204</v>
+        <v>156</v>
       </c>
       <c r="AO8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AX8" t="s">
-        <v>229</v>
-      </c>
-      <c r="AY8" t="s">
-        <v>230</v>
-      </c>
-      <c r="AZ8" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="BB8" t="s">
-        <v>245</v>
-      </c>
-      <c r="BD8" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="BF8" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="BG8" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:59">
@@ -2184,55 +2157,34 @@
         <v>66</v>
       </c>
       <c r="B9" s="2">
-        <v>46004.72183795925</v>
-      </c>
-      <c r="J9" t="s">
-        <v>100</v>
+        <v>46004.70114318176</v>
       </c>
       <c r="S9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="T9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="V9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="W9" t="s">
         <v>155</v>
       </c>
-      <c r="AA9" t="s">
-        <v>172</v>
-      </c>
-      <c r="AJ9" t="s">
-        <v>194</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>205</v>
-      </c>
       <c r="AO9" t="s">
         <v>155</v>
       </c>
       <c r="AX9" t="s">
-        <v>229</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>231</v>
-      </c>
-      <c r="AZ9" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="BB9" t="s">
-        <v>245</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="BF9" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="BG9" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:59">
@@ -2240,58 +2192,55 @@
         <v>67</v>
       </c>
       <c r="B10" s="2">
-        <v>46004.72183795925</v>
+        <v>46004.72246635323</v>
       </c>
       <c r="J10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="S10" t="s">
         <v>125</v>
       </c>
       <c r="T10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="V10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="W10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="AA10" t="s">
-        <v>171</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="AJ10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AM10" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AO10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="AX10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AY10" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="AZ10" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="BB10" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="BD10" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="BF10" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="BG10" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:59">
@@ -2299,58 +2248,58 @@
         <v>68</v>
       </c>
       <c r="B11" s="2">
-        <v>46004.72183795925</v>
+        <v>46004.72246635323</v>
       </c>
       <c r="J11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="S11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="V11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="W11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AA11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="AD11" t="s">
         <v>178</v>
       </c>
       <c r="AJ11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AM11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AO11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="AX11" t="s">
+        <v>227</v>
+      </c>
+      <c r="AY11" t="s">
         <v>229</v>
       </c>
-      <c r="AY11" t="s">
-        <v>233</v>
-      </c>
       <c r="AZ11" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="BB11" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="BD11" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="BF11" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="BG11" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Excel export by removing timezone from datetime columns
</commit_message>
<xml_diff>
--- a/output/user_output.xlsx
+++ b/output/user_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="277">
   <si>
     <t>part_number</t>
   </si>
@@ -313,6 +313,15 @@
     <t>2096.8</t>
   </si>
   <si>
+    <t>1683.78</t>
+  </si>
+  <si>
+    <t>1428.22</t>
+  </si>
+  <si>
+    <t>16.41</t>
+  </si>
+  <si>
     <t>2787.32</t>
   </si>
   <si>
@@ -550,6 +559,15 @@
     <t>Checked In</t>
   </si>
   <si>
+    <t>Standard Order</t>
+  </si>
+  <si>
+    <t>Check Material Cert</t>
+  </si>
+  <si>
+    <t>Urgent</t>
+  </si>
+  <si>
     <t>Warranty Included</t>
   </si>
   <si>
@@ -598,6 +616,15 @@
     <t>4.46</t>
   </si>
   <si>
+    <t>PO1003</t>
+  </si>
+  <si>
+    <t>PO1004</t>
+  </si>
+  <si>
+    <t>PO1005</t>
+  </si>
+  <si>
     <t>INV2002</t>
   </si>
   <si>
@@ -625,6 +652,15 @@
     <t>SL20</t>
   </si>
   <si>
+    <t>471</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>445</t>
+  </si>
+  <si>
     <t>275</t>
   </si>
   <si>
@@ -697,6 +733,24 @@
     <t>28.0</t>
   </si>
   <si>
+    <t>2024-02-10</t>
+  </si>
+  <si>
+    <t>2024-11-13</t>
+  </si>
+  <si>
+    <t>2024-11-08</t>
+  </si>
+  <si>
+    <t>2024-04-11</t>
+  </si>
+  <si>
+    <t>2024-09-13</t>
+  </si>
+  <si>
+    <t>2024-02-25</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
@@ -730,10 +784,7 @@
     <t>[{"source_system": "sap", "source_file": "sap_master_mock.xlsx"}, {"source_system": "vault", "source_file": "vault_mock_aligned.xlsx"}, {"source_system": "powerbi", "source_file": "powerbi_mock_aligned.xlsx"}, {"source_system": "user", "source_file": "diagram2.pdf"}]</t>
   </si>
   <si>
-    <t>[{"source": "user", "file": "diagram 7.pdf", "description": "Steel Screw 39x90 mm"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source": "user", "file": "diagram 7.pdf", "description": "Steel Screw 39x90 mm"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source": "user", "file": "diagram 7.pdf", "description": "Steel Screw 39x90 mm"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}]</t>
-  </si>
-  <si>
-    <t>[{"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}]</t>
+    <t>[{"source_system": "pos", "source_file": "po_mock_newparts.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}]</t>
   </si>
   <si>
     <t>[{"source_system": "invoices", "source_file": "invoice_mock_newparts.pdf"}, {"source_system": "user", "source_file": "diagram2.pdf"}]</t>
@@ -758,6 +809,15 @@
   </si>
   <si>
     <t>ABC Industries</t>
+  </si>
+  <si>
+    <t>MegaTools Pvt Ltd</t>
+  </si>
+  <si>
+    <t>ElectroMart</t>
+  </si>
+  <si>
+    <t>UniMach</t>
   </si>
   <si>
     <t>Alpha Metals</t>
@@ -1336,7 +1396,7 @@
         <v>59</v>
       </c>
       <c r="B2" s="2">
-        <v>46004.72246635323</v>
+        <v>46028.67361742735</v>
       </c>
       <c r="C2" t="s">
         <v>69</v>
@@ -1360,124 +1420,124 @@
         <v>94</v>
       </c>
       <c r="K2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="L2" t="s">
+        <v>107</v>
+      </c>
+      <c r="M2" t="s">
+        <v>110</v>
+      </c>
+      <c r="N2" t="s">
+        <v>115</v>
+      </c>
+      <c r="O2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P2" t="s">
         <v>104</v>
       </c>
-      <c r="M2" t="s">
-        <v>107</v>
-      </c>
-      <c r="N2" t="s">
-        <v>112</v>
-      </c>
-      <c r="O2" t="s">
-        <v>117</v>
-      </c>
-      <c r="P2" t="s">
-        <v>101</v>
-      </c>
       <c r="Q2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="R2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="S2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="T2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="U2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="V2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="W2" t="s">
         <v>90</v>
       </c>
       <c r="X2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="Y2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="Z2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AA2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="AB2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AC2" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AE2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="AF2" t="s">
         <v>80</v>
       </c>
       <c r="AG2" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="AI2" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="AK2" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="AL2" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="AO2" t="s">
         <v>90</v>
       </c>
       <c r="AP2" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="AQ2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AR2" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="AS2" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="AT2" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="AU2" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="AX2" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="BA2" t="s">
-        <v>232</v>
+        <v>250</v>
       </c>
       <c r="BB2" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="BC2" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="BD2" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="BE2" t="s">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c r="BF2" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="BG2" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:59">
@@ -1485,7 +1545,7 @@
         <v>60</v>
       </c>
       <c r="B3" s="2">
-        <v>46004.72246635323</v>
+        <v>46028.67361742735</v>
       </c>
       <c r="C3" t="s">
         <v>70</v>
@@ -1512,124 +1572,124 @@
         <v>95</v>
       </c>
       <c r="K3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="M3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="N3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="O3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="P3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="Q3" t="s">
+        <v>123</v>
+      </c>
+      <c r="R3" t="s">
+        <v>126</v>
+      </c>
+      <c r="S3" t="s">
+        <v>128</v>
+      </c>
+      <c r="T3" t="s">
+        <v>133</v>
+      </c>
+      <c r="U3" t="s">
+        <v>143</v>
+      </c>
+      <c r="V3" t="s">
+        <v>148</v>
+      </c>
+      <c r="W3" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>179</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>188</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>190</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>192</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>196</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>206</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>208</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>217</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>157</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>221</v>
+      </c>
+      <c r="AQ3" t="s">
         <v>120</v>
       </c>
-      <c r="R3" t="s">
-        <v>123</v>
-      </c>
-      <c r="S3" t="s">
-        <v>125</v>
-      </c>
-      <c r="T3" t="s">
-        <v>130</v>
-      </c>
-      <c r="U3" t="s">
-        <v>140</v>
-      </c>
-      <c r="V3" t="s">
-        <v>145</v>
-      </c>
-      <c r="W3" t="s">
-        <v>154</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>168</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>172</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>176</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>180</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>184</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>186</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>190</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>197</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>199</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>205</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>154</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>209</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>117</v>
-      </c>
       <c r="AR3" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="AS3" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="AT3" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="AU3" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="AX3" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="BA3" t="s">
-        <v>233</v>
+        <v>251</v>
       </c>
       <c r="BB3" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="BC3" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="BD3" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="BE3" t="s">
-        <v>251</v>
+        <v>271</v>
       </c>
       <c r="BF3" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="BG3" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:59">
@@ -1637,7 +1697,7 @@
         <v>61</v>
       </c>
       <c r="B4" s="2">
-        <v>46004.72246635323</v>
+        <v>46028.67361742735</v>
       </c>
       <c r="C4" t="s">
         <v>71</v>
@@ -1664,121 +1724,121 @@
         <v>96</v>
       </c>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L4" t="s">
+        <v>108</v>
+      </c>
+      <c r="M4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" t="s">
+        <v>117</v>
+      </c>
+      <c r="O4" t="s">
+        <v>120</v>
+      </c>
+      <c r="P4" t="s">
         <v>105</v>
       </c>
-      <c r="M4" t="s">
-        <v>109</v>
-      </c>
-      <c r="N4" t="s">
-        <v>114</v>
-      </c>
-      <c r="O4" t="s">
-        <v>117</v>
-      </c>
-      <c r="P4" t="s">
-        <v>102</v>
-      </c>
       <c r="Q4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="S4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="T4" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="U4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="V4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="W4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="X4" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="Y4" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="Z4" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="AA4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="AB4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AC4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AE4" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="AF4" t="s">
         <v>79</v>
       </c>
       <c r="AG4" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="AI4" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="AK4" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="AL4" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="AN4" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="AO4" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="AP4" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="AQ4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AR4" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="AS4" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="AT4" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="AX4" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="BA4" t="s">
-        <v>234</v>
+        <v>252</v>
       </c>
       <c r="BB4" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="BC4" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="BD4" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="BE4" t="s">
-        <v>252</v>
+        <v>272</v>
       </c>
       <c r="BF4" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="BG4" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:59">
@@ -1786,7 +1846,7 @@
         <v>62</v>
       </c>
       <c r="B5" s="2">
-        <v>46004.72246635323</v>
+        <v>46028.67361742735</v>
       </c>
       <c r="C5" t="s">
         <v>72</v>
@@ -1813,127 +1873,127 @@
         <v>97</v>
       </c>
       <c r="K5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="L5" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="M5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="N5" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="O5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="P5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="Q5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="R5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="S5" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="T5" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="U5" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="V5" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="W5" t="s">
         <v>92</v>
       </c>
       <c r="X5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="Y5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="Z5" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="AA5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="AB5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AC5" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AE5" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="AF5" t="s">
         <v>79</v>
       </c>
       <c r="AG5" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="AH5" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="AI5" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="AK5" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="AL5" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="AN5" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="AO5" t="s">
         <v>92</v>
       </c>
       <c r="AP5" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="AQ5" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AR5" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="AS5" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="AT5" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="AX5" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="BA5" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="BB5" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="BC5" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="BD5" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="BE5" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
       <c r="BF5" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="BG5" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:59">
@@ -1941,7 +2001,7 @@
         <v>63</v>
       </c>
       <c r="B6" s="2">
-        <v>46004.72246635323</v>
+        <v>46028.67361742735</v>
       </c>
       <c r="C6" t="s">
         <v>73</v>
@@ -1965,121 +2025,121 @@
         <v>98</v>
       </c>
       <c r="K6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="L6" t="s">
+        <v>108</v>
+      </c>
+      <c r="M6" t="s">
+        <v>114</v>
+      </c>
+      <c r="N6" t="s">
+        <v>119</v>
+      </c>
+      <c r="O6" t="s">
+        <v>120</v>
+      </c>
+      <c r="P6" t="s">
         <v>105</v>
       </c>
-      <c r="M6" t="s">
-        <v>111</v>
-      </c>
-      <c r="N6" t="s">
-        <v>116</v>
-      </c>
-      <c r="O6" t="s">
-        <v>117</v>
-      </c>
-      <c r="P6" t="s">
-        <v>102</v>
-      </c>
       <c r="Q6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="S6" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="T6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="U6" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="V6" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="W6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="X6" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="Y6" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="Z6" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AA6" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="AB6" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="AC6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AE6" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="AF6" t="s">
         <v>80</v>
       </c>
       <c r="AG6" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="AH6" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="AI6" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="AK6" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="AL6" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="AO6" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="AP6" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="AQ6" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="AR6" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="AS6" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="AT6" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="AX6" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="BA6" t="s">
-        <v>236</v>
+        <v>254</v>
       </c>
       <c r="BB6" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="BC6" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="BD6" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="BE6" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="BF6" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="BG6" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:59">
@@ -2087,34 +2147,58 @@
         <v>64</v>
       </c>
       <c r="B7" s="2">
-        <v>46004.70114318176</v>
+        <v>46028.67361742735</v>
+      </c>
+      <c r="J7" t="s">
+        <v>99</v>
       </c>
       <c r="S7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="T7" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="V7" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="W7" t="s">
-        <v>154</v>
+        <v>157</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>181</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>200</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>212</v>
       </c>
       <c r="AO7" t="s">
-        <v>154</v>
+        <v>157</v>
+      </c>
+      <c r="AV7" t="s">
+        <v>239</v>
+      </c>
+      <c r="AW7" t="s">
+        <v>242</v>
       </c>
       <c r="AX7" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="BB7" t="s">
-        <v>238</v>
+        <v>256</v>
+      </c>
+      <c r="BD7" t="s">
+        <v>265</v>
       </c>
       <c r="BF7" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="BG7" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="8" spans="1:59">
@@ -2122,34 +2206,58 @@
         <v>65</v>
       </c>
       <c r="B8" s="2">
-        <v>46004.70114318176</v>
+        <v>46028.67361742735</v>
+      </c>
+      <c r="J8" t="s">
+        <v>100</v>
       </c>
       <c r="S8" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="T8" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="V8" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="W8" t="s">
-        <v>156</v>
+        <v>159</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>176</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>213</v>
       </c>
       <c r="AO8" t="s">
-        <v>156</v>
+        <v>159</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>240</v>
+      </c>
+      <c r="AW8" t="s">
+        <v>243</v>
       </c>
       <c r="AX8" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="BB8" t="s">
-        <v>239</v>
+        <v>256</v>
+      </c>
+      <c r="BD8" t="s">
+        <v>266</v>
       </c>
       <c r="BF8" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="BG8" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:59">
@@ -2157,34 +2265,58 @@
         <v>66</v>
       </c>
       <c r="B9" s="2">
-        <v>46004.70114318176</v>
+        <v>46028.67361742735</v>
+      </c>
+      <c r="J9" t="s">
+        <v>101</v>
       </c>
       <c r="S9" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="T9" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="V9" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="W9" t="s">
-        <v>155</v>
+        <v>158</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>176</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>183</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>202</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>214</v>
       </c>
       <c r="AO9" t="s">
-        <v>155</v>
+        <v>158</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>241</v>
+      </c>
+      <c r="AW9" t="s">
+        <v>244</v>
       </c>
       <c r="AX9" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="BB9" t="s">
-        <v>239</v>
+        <v>256</v>
+      </c>
+      <c r="BD9" t="s">
+        <v>267</v>
       </c>
       <c r="BF9" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="BG9" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:59">
@@ -2192,55 +2324,55 @@
         <v>67</v>
       </c>
       <c r="B10" s="2">
-        <v>46004.72246635323</v>
+        <v>46028.67361742735</v>
       </c>
       <c r="J10" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="S10" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="T10" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="V10" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="W10" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AA10" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AJ10" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="AM10" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="AO10" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="AX10" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="AY10" t="s">
-        <v>228</v>
+        <v>246</v>
       </c>
       <c r="AZ10" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="BB10" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="BD10" t="s">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c r="BF10" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="BG10" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:59">
@@ -2248,58 +2380,58 @@
         <v>68</v>
       </c>
       <c r="B11" s="2">
-        <v>46004.72246635323</v>
+        <v>46028.67361742735</v>
       </c>
       <c r="J11" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="S11" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="T11" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="V11" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="W11" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AA11" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="AD11" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="AJ11" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="AM11" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="AO11" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="AX11" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="AY11" t="s">
-        <v>229</v>
+        <v>247</v>
       </c>
       <c r="AZ11" t="s">
-        <v>231</v>
+        <v>249</v>
       </c>
       <c r="BB11" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="BD11" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="BF11" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="BG11" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>